<commit_message>
Added frontend and .gitignore file
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="31560" yWindow="-4420" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Change Sets" sheetId="2" r:id="rId2"/>
+    <sheet name="Frontend" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Phase 1</t>
   </si>
@@ -104,6 +105,12 @@
   </si>
   <si>
     <t>Dynamic content rendering from EP Engine</t>
+  </si>
+  <si>
+    <t>Setup Info</t>
+  </si>
+  <si>
+    <t>Maven Frontend Goal</t>
   </si>
 </sst>
 </file>
@@ -555,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -753,4 +760,32 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change set details added
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="-4420" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Phase 1</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Maven Frontend Goal</t>
+  </si>
+  <si>
+    <t>Page 1</t>
+  </si>
+  <si>
+    <t>All pages</t>
   </si>
 </sst>
 </file>
@@ -744,15 +750,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -766,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>